<commit_message>
added plots for flower sales from april until june
</commit_message>
<xml_diff>
--- a/april_june.xlsx
+++ b/april_june.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Holex\Desktop\Stats_Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="3860" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="7500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,6 +164,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -486,29 +499,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -593,7 +606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -637,7 +650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -681,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -725,7 +738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -769,7 +782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -813,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -857,7 +870,7 @@
         <v>-4.99</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -901,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -945,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -989,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1033,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1077,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1121,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1165,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1209,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1253,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1341,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1385,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1429,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1473,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1517,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1561,7 +1574,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1605,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1649,7 +1662,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1693,7 +1706,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1737,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1781,7 +1794,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -1825,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
@@ -1869,7 +1882,7 @@
         <v>-95.99</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
@@ -1913,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>13</v>
       </c>
@@ -1957,7 +1970,7 @@
         <v>-149.94999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>13</v>
       </c>
@@ -2001,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
@@ -2045,7 +2058,7 @@
         <v>-249.9</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>13</v>
       </c>
@@ -2089,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>13</v>
       </c>
@@ -2133,7 +2146,7 @@
         <v>-182.2</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>13</v>
       </c>
@@ -2177,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>13</v>
       </c>
@@ -2221,7 +2234,7 @@
         <v>-200.15</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>13</v>
       </c>
@@ -2265,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>13</v>
       </c>
@@ -2309,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -2353,7 +2366,7 @@
         <v>-103.99</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
@@ -2397,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>13</v>
       </c>
@@ -2441,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>13</v>
       </c>
@@ -2485,7 +2498,7 @@
         <v>-144.19</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>13</v>
       </c>
@@ -2529,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>13</v>
       </c>
@@ -2573,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>13</v>
       </c>
@@ -2617,7 +2630,7 @@
         <v>-203.19</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>13</v>
       </c>
@@ -2661,7 +2674,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>13</v>
       </c>
@@ -2705,7 +2718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>13</v>
       </c>
@@ -2749,7 +2762,7 @@
         <v>-193.99</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>13</v>
       </c>
@@ -2793,7 +2806,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>13</v>
       </c>
@@ -2837,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>13</v>
       </c>
@@ -2881,7 +2894,7 @@
         <v>-322.67</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>13</v>
       </c>
@@ -2925,7 +2938,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>13</v>
       </c>
@@ -2969,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>13</v>
       </c>
@@ -3013,7 +3026,7 @@
         <v>-226</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>13</v>
       </c>
@@ -3057,7 +3070,7 @@
         <v>-6.99</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>13</v>
       </c>
@@ -3101,7 +3114,7 @@
         <v>-190.96</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>13</v>
       </c>
@@ -3145,7 +3158,7 @@
         <v>-19.899999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>13</v>
       </c>
@@ -3189,7 +3202,7 @@
         <v>-93</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>13</v>
       </c>
@@ -3233,7 +3246,7 @@
         <v>-15.92</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>13</v>
       </c>
@@ -3277,7 +3290,7 @@
         <v>-66.989999999999995</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>13</v>
       </c>
@@ -3321,7 +3334,7 @@
         <v>-3.98</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>13</v>
       </c>
@@ -3365,7 +3378,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>13</v>
       </c>
@@ -3409,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>13</v>
       </c>
@@ -3453,7 +3466,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>13</v>
       </c>
@@ -3497,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>13</v>
       </c>
@@ -3541,7 +3554,7 @@
         <v>-3.98</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>13</v>
       </c>
@@ -3585,7 +3598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>13</v>
       </c>
@@ -3629,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>13</v>
       </c>
@@ -3673,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>13</v>
       </c>
@@ -3717,7 +3730,7 @@
         <v>-32</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>13</v>
       </c>
@@ -3761,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>13</v>
       </c>
@@ -3805,7 +3818,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>13</v>
       </c>
@@ -3849,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>13</v>
       </c>
@@ -3893,7 +3906,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>13</v>
       </c>
@@ -3937,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>13</v>
       </c>
@@ -3981,7 +3994,7 @@
         <v>-49.98</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>13</v>
       </c>
@@ -4025,7 +4038,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>13</v>
       </c>
@@ -4069,7 +4082,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>13</v>
       </c>
@@ -4113,7 +4126,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>13</v>
       </c>
@@ -4157,7 +4170,7 @@
         <v>-49.97</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>13</v>
       </c>
@@ -4201,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>13</v>
       </c>
@@ -4245,7 +4258,7 @@
         <v>-93.94</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>13</v>
       </c>
@@ -4289,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>13</v>
       </c>
@@ -4333,7 +4346,7 @@
         <v>-3.98</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>13</v>
       </c>
@@ -4377,7 +4390,7 @@
         <v>-33.979999999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>13</v>
       </c>
@@ -4421,7 +4434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>13</v>
       </c>
@@ -4465,7 +4478,7 @@
         <v>-10.64</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>13</v>
       </c>
@@ -4509,7 +4522,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>13</v>
       </c>
@@ -4553,7 +4566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>13</v>
       </c>
@@ -4597,7 +4610,7 @@
         <v>-12.99</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>13</v>
       </c>
@@ -4641,7 +4654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>13</v>
       </c>
@@ -4685,7 +4698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>13</v>
       </c>
@@ -4729,7 +4742,7 @@
         <v>-22.99</v>
       </c>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>13</v>
       </c>
@@ -4773,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>13</v>
       </c>
@@ -4817,7 +4830,7 @@
         <v>-19.95</v>
       </c>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>13</v>
       </c>
@@ -4861,7 +4874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>13</v>
       </c>
@@ -4905,7 +4918,7 @@
         <v>-13.96</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>13</v>
       </c>
@@ -4949,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>13</v>
       </c>
@@ -4993,7 +5006,7 @@
         <v>-30.41</v>
       </c>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>13</v>
       </c>
@@ -5037,7 +5050,7 @@
         <v>-17.989999999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>13</v>
       </c>
@@ -5081,7 +5094,7 @@
         <v>-27.92</v>
       </c>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>13</v>
       </c>
@@ -5125,7 +5138,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>13</v>
       </c>
@@ -5169,7 +5182,7 @@
         <v>-55.84</v>
       </c>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>13</v>
       </c>
@@ -5213,7 +5226,7 @@
         <v>-22.99</v>
       </c>
     </row>
-    <row r="108" spans="1:14">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>13</v>
       </c>
@@ -5257,7 +5270,7 @@
         <v>-20.47</v>
       </c>
     </row>
-    <row r="109" spans="1:14">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>13</v>
       </c>
@@ -5301,7 +5314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:14">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>13</v>
       </c>
@@ -5345,7 +5358,7 @@
         <v>-27.92</v>
       </c>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>13</v>
       </c>
@@ -5389,7 +5402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:14">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>13</v>
       </c>
@@ -5433,7 +5446,7 @@
         <v>-15.47</v>
       </c>
     </row>
-    <row r="113" spans="1:14">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>13</v>
       </c>
@@ -5477,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>13</v>
       </c>
@@ -5521,7 +5534,7 @@
         <v>-14.47</v>
       </c>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>13</v>
       </c>
@@ -5565,7 +5578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>13</v>
       </c>
@@ -5609,7 +5622,7 @@
         <v>-3.49</v>
       </c>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>13</v>
       </c>
@@ -5653,7 +5666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>13</v>
       </c>
@@ -5697,7 +5710,7 @@
         <v>-6.98</v>
       </c>
     </row>
-    <row r="119" spans="1:14">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>13</v>
       </c>
@@ -5741,7 +5754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>13</v>
       </c>
@@ -5785,7 +5798,7 @@
         <v>-24.43</v>
       </c>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>13</v>
       </c>
@@ -5829,7 +5842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>13</v>
       </c>
@@ -5873,7 +5886,7 @@
         <v>-659.35</v>
       </c>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>13</v>
       </c>
@@ -5917,7 +5930,7 @@
         <v>-8.99</v>
       </c>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>13</v>
       </c>
@@ -5961,7 +5974,7 @@
         <v>-63</v>
       </c>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>13</v>
       </c>
@@ -6005,7 +6018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:14">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>13</v>
       </c>
@@ -6049,7 +6062,7 @@
         <v>-33</v>
       </c>
     </row>
-    <row r="127" spans="1:14">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>13</v>
       </c>
@@ -6093,7 +6106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:14">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>13</v>
       </c>
@@ -6137,7 +6150,7 @@
         <v>-38.94</v>
       </c>
     </row>
-    <row r="129" spans="1:14">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>13</v>
       </c>
@@ -6181,7 +6194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:14">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>13</v>
       </c>
@@ -6225,7 +6238,7 @@
         <v>-71.94</v>
       </c>
     </row>
-    <row r="131" spans="1:14">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>13</v>
       </c>
@@ -6269,7 +6282,7 @@
         <v>-8.99</v>
       </c>
     </row>
-    <row r="132" spans="1:14">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>13</v>
       </c>
@@ -6313,7 +6326,7 @@
         <v>-70</v>
       </c>
     </row>
-    <row r="133" spans="1:14">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>13</v>
       </c>
@@ -6357,7 +6370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:14">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>13</v>
       </c>
@@ -6401,7 +6414,7 @@
         <v>-167.94</v>
       </c>
     </row>
-    <row r="135" spans="1:14">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>13</v>
       </c>
@@ -6445,7 +6458,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="136" spans="1:14">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>13</v>
       </c>
@@ -6489,7 +6502,7 @@
         <v>-6.99</v>
       </c>
     </row>
-    <row r="137" spans="1:14">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>13</v>
       </c>
@@ -6533,7 +6546,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="138" spans="1:14">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>13</v>
       </c>
@@ -6577,7 +6590,7 @@
         <v>-18.98</v>
       </c>
     </row>
-    <row r="139" spans="1:14">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>13</v>
       </c>
@@ -6621,7 +6634,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="140" spans="1:14">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="3"/>
       <c r="C140" s="2"/>
@@ -6637,7 +6650,7 @@
       <c r="M140" s="2"/>
       <c r="N140" s="2"/>
     </row>
-    <row r="141" spans="1:14">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="3"/>
       <c r="C141" s="2"/>
@@ -6653,7 +6666,7 @@
       <c r="M141" s="2"/>
       <c r="N141" s="2"/>
     </row>
-    <row r="142" spans="1:14">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="3"/>
       <c r="C142" s="2"/>
@@ -6669,7 +6682,7 @@
       <c r="M142" s="2"/>
       <c r="N142" s="2"/>
     </row>
-    <row r="143" spans="1:14">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="3"/>
       <c r="C143" s="2"/>
@@ -6685,7 +6698,7 @@
       <c r="M143" s="2"/>
       <c r="N143" s="2"/>
     </row>
-    <row r="144" spans="1:14">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="3"/>
       <c r="C144" s="2"/>
@@ -6701,7 +6714,7 @@
       <c r="M144" s="2"/>
       <c r="N144" s="2"/>
     </row>
-    <row r="145" spans="1:14">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="3"/>
       <c r="C145" s="2"/>
@@ -6717,7 +6730,7 @@
       <c r="M145" s="2"/>
       <c r="N145" s="2"/>
     </row>
-    <row r="146" spans="1:14">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="3"/>
       <c r="C146" s="2"/>
@@ -6733,7 +6746,7 @@
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
     </row>
-    <row r="147" spans="1:14">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="2"/>
@@ -6749,7 +6762,7 @@
       <c r="M147" s="2"/>
       <c r="N147" s="2"/>
     </row>
-    <row r="148" spans="1:14">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="2"/>
@@ -6765,7 +6778,7 @@
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
     </row>
-    <row r="149" spans="1:14">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="3"/>
       <c r="C149" s="2"/>
@@ -6781,7 +6794,7 @@
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
     </row>
-    <row r="150" spans="1:14">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="3"/>
       <c r="C150" s="2"/>
@@ -6797,7 +6810,7 @@
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
     </row>
-    <row r="151" spans="1:14">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="3"/>
       <c r="C151" s="2"/>
@@ -6813,7 +6826,7 @@
       <c r="M151" s="2"/>
       <c r="N151" s="2"/>
     </row>
-    <row r="152" spans="1:14">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="3"/>
       <c r="C152" s="2"/>
@@ -6829,7 +6842,7 @@
       <c r="M152" s="2"/>
       <c r="N152" s="2"/>
     </row>
-    <row r="153" spans="1:14">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="3"/>
       <c r="C153" s="2"/>
@@ -6845,7 +6858,7 @@
       <c r="M153" s="2"/>
       <c r="N153" s="2"/>
     </row>
-    <row r="154" spans="1:14">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="3"/>
       <c r="C154" s="2"/>
@@ -6861,7 +6874,7 @@
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
     </row>
-    <row r="155" spans="1:14">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="3"/>
       <c r="C155" s="2"/>
@@ -6877,7 +6890,7 @@
       <c r="M155" s="2"/>
       <c r="N155" s="2"/>
     </row>
-    <row r="156" spans="1:14">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="3"/>
       <c r="C156" s="2"/>
@@ -6893,7 +6906,7 @@
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
     </row>
-    <row r="157" spans="1:14">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="3"/>
       <c r="C157" s="2"/>
@@ -6909,7 +6922,7 @@
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
     </row>
-    <row r="158" spans="1:14">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="3"/>
       <c r="C158" s="2"/>
@@ -6925,7 +6938,7 @@
       <c r="M158" s="2"/>
       <c r="N158" s="2"/>
     </row>
-    <row r="159" spans="1:14">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
       <c r="B159" s="3"/>
       <c r="C159" s="2"/>
@@ -6941,7 +6954,7 @@
       <c r="M159" s="2"/>
       <c r="N159" s="2"/>
     </row>
-    <row r="160" spans="1:14">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="3"/>
       <c r="C160" s="2"/>
@@ -6957,7 +6970,7 @@
       <c r="M160" s="2"/>
       <c r="N160" s="2"/>
     </row>
-    <row r="161" spans="1:14">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A161" s="2"/>
       <c r="B161" s="3"/>
       <c r="C161" s="2"/>
@@ -6973,7 +6986,7 @@
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
     </row>
-    <row r="162" spans="1:14">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A162" s="2"/>
       <c r="B162" s="3"/>
       <c r="C162" s="2"/>
@@ -6989,7 +7002,7 @@
       <c r="M162" s="2"/>
       <c r="N162" s="2"/>
     </row>
-    <row r="163" spans="1:14">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
       <c r="B163" s="3"/>
       <c r="C163" s="2"/>
@@ -7005,7 +7018,7 @@
       <c r="M163" s="2"/>
       <c r="N163" s="2"/>
     </row>
-    <row r="164" spans="1:14">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A164" s="2"/>
       <c r="B164" s="3"/>
       <c r="C164" s="2"/>
@@ -7021,7 +7034,7 @@
       <c r="M164" s="2"/>
       <c r="N164" s="2"/>
     </row>
-    <row r="165" spans="1:14">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A165" s="2"/>
       <c r="B165" s="3"/>
       <c r="C165" s="2"/>
@@ -7037,7 +7050,7 @@
       <c r="M165" s="2"/>
       <c r="N165" s="2"/>
     </row>
-    <row r="166" spans="1:14">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A166" s="2"/>
       <c r="B166" s="3"/>
       <c r="C166" s="2"/>
@@ -7053,7 +7066,7 @@
       <c r="M166" s="2"/>
       <c r="N166" s="2"/>
     </row>
-    <row r="167" spans="1:14">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A167" s="2"/>
       <c r="B167" s="3"/>
       <c r="C167" s="2"/>
@@ -7069,7 +7082,7 @@
       <c r="M167" s="2"/>
       <c r="N167" s="2"/>
     </row>
-    <row r="168" spans="1:14">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A168" s="2"/>
       <c r="B168" s="3"/>
       <c r="C168" s="2"/>
@@ -7085,7 +7098,7 @@
       <c r="M168" s="2"/>
       <c r="N168" s="2"/>
     </row>
-    <row r="169" spans="1:14">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A169" s="2"/>
       <c r="B169" s="3"/>
       <c r="C169" s="2"/>
@@ -7101,7 +7114,7 @@
       <c r="M169" s="2"/>
       <c r="N169" s="2"/>
     </row>
-    <row r="170" spans="1:14">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A170" s="2"/>
       <c r="B170" s="3"/>
       <c r="C170" s="2"/>
@@ -7117,7 +7130,7 @@
       <c r="M170" s="2"/>
       <c r="N170" s="2"/>
     </row>
-    <row r="171" spans="1:14">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A171" s="2"/>
       <c r="B171" s="3"/>
       <c r="C171" s="2"/>
@@ -7133,7 +7146,7 @@
       <c r="M171" s="2"/>
       <c r="N171" s="2"/>
     </row>
-    <row r="172" spans="1:14">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A172" s="2"/>
       <c r="B172" s="3"/>
       <c r="C172" s="2"/>
@@ -7149,7 +7162,7 @@
       <c r="M172" s="2"/>
       <c r="N172" s="2"/>
     </row>
-    <row r="173" spans="1:14">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A173" s="2"/>
       <c r="B173" s="3"/>
       <c r="C173" s="2"/>
@@ -7165,7 +7178,7 @@
       <c r="M173" s="2"/>
       <c r="N173" s="2"/>
     </row>
-    <row r="174" spans="1:14">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A174" s="2"/>
       <c r="B174" s="3"/>
       <c r="C174" s="2"/>
@@ -7181,7 +7194,7 @@
       <c r="M174" s="2"/>
       <c r="N174" s="2"/>
     </row>
-    <row r="175" spans="1:14">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A175" s="2"/>
       <c r="B175" s="3"/>
       <c r="C175" s="2"/>
@@ -7197,7 +7210,7 @@
       <c r="M175" s="2"/>
       <c r="N175" s="2"/>
     </row>
-    <row r="176" spans="1:14">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A176" s="2"/>
       <c r="B176" s="3"/>
       <c r="C176" s="2"/>
@@ -7213,7 +7226,7 @@
       <c r="M176" s="2"/>
       <c r="N176" s="2"/>
     </row>
-    <row r="177" spans="1:14">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A177" s="2"/>
       <c r="B177" s="3"/>
       <c r="C177" s="2"/>
@@ -7229,7 +7242,7 @@
       <c r="M177" s="2"/>
       <c r="N177" s="2"/>
     </row>
-    <row r="178" spans="1:14">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A178" s="2"/>
       <c r="B178" s="3"/>
       <c r="C178" s="2"/>
@@ -7245,7 +7258,7 @@
       <c r="M178" s="2"/>
       <c r="N178" s="2"/>
     </row>
-    <row r="179" spans="1:14">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A179" s="2"/>
       <c r="B179" s="3"/>
       <c r="C179" s="2"/>
@@ -7261,7 +7274,7 @@
       <c r="M179" s="2"/>
       <c r="N179" s="2"/>
     </row>
-    <row r="180" spans="1:14">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A180" s="2"/>
       <c r="B180" s="3"/>
       <c r="C180" s="2"/>
@@ -7277,7 +7290,7 @@
       <c r="M180" s="2"/>
       <c r="N180" s="2"/>
     </row>
-    <row r="181" spans="1:14">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A181" s="2"/>
       <c r="B181" s="3"/>
       <c r="C181" s="2"/>
@@ -7293,7 +7306,7 @@
       <c r="M181" s="2"/>
       <c r="N181" s="2"/>
     </row>
-    <row r="182" spans="1:14">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A182" s="2"/>
       <c r="B182" s="3"/>
       <c r="C182" s="2"/>
@@ -7309,7 +7322,7 @@
       <c r="M182" s="2"/>
       <c r="N182" s="2"/>
     </row>
-    <row r="183" spans="1:14">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A183" s="2"/>
       <c r="B183" s="3"/>
       <c r="C183" s="2"/>
@@ -7325,7 +7338,7 @@
       <c r="M183" s="2"/>
       <c r="N183" s="2"/>
     </row>
-    <row r="184" spans="1:14">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A184" s="2"/>
       <c r="B184" s="3"/>
       <c r="C184" s="2"/>
@@ -7341,7 +7354,7 @@
       <c r="M184" s="2"/>
       <c r="N184" s="2"/>
     </row>
-    <row r="185" spans="1:14">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A185" s="2"/>
       <c r="B185" s="3"/>
       <c r="C185" s="2"/>
@@ -7357,7 +7370,7 @@
       <c r="M185" s="2"/>
       <c r="N185" s="2"/>
     </row>
-    <row r="186" spans="1:14">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A186" s="2"/>
       <c r="B186" s="3"/>
       <c r="C186" s="2"/>
@@ -7373,7 +7386,7 @@
       <c r="M186" s="2"/>
       <c r="N186" s="2"/>
     </row>
-    <row r="187" spans="1:14">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A187" s="2"/>
       <c r="B187" s="3"/>
       <c r="C187" s="2"/>
@@ -7389,7 +7402,7 @@
       <c r="M187" s="2"/>
       <c r="N187" s="2"/>
     </row>
-    <row r="188" spans="1:14">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A188" s="2"/>
       <c r="B188" s="3"/>
       <c r="C188" s="2"/>
@@ -7405,7 +7418,7 @@
       <c r="M188" s="2"/>
       <c r="N188" s="2"/>
     </row>
-    <row r="189" spans="1:14">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A189" s="2"/>
       <c r="B189" s="3"/>
       <c r="C189" s="2"/>
@@ -7421,7 +7434,7 @@
       <c r="M189" s="2"/>
       <c r="N189" s="2"/>
     </row>
-    <row r="190" spans="1:14">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A190" s="2"/>
       <c r="B190" s="3"/>
       <c r="C190" s="2"/>
@@ -7437,7 +7450,7 @@
       <c r="M190" s="2"/>
       <c r="N190" s="2"/>
     </row>
-    <row r="191" spans="1:14">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A191" s="2"/>
       <c r="B191" s="3"/>
       <c r="C191" s="2"/>
@@ -7453,7 +7466,7 @@
       <c r="M191" s="2"/>
       <c r="N191" s="2"/>
     </row>
-    <row r="192" spans="1:14">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A192" s="2"/>
       <c r="B192" s="3"/>
       <c r="C192" s="2"/>
@@ -7469,7 +7482,7 @@
       <c r="M192" s="2"/>
       <c r="N192" s="2"/>
     </row>
-    <row r="193" spans="1:14">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A193" s="2"/>
       <c r="B193" s="3"/>
       <c r="C193" s="2"/>
@@ -7485,7 +7498,7 @@
       <c r="M193" s="2"/>
       <c r="N193" s="2"/>
     </row>
-    <row r="194" spans="1:14">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A194" s="2"/>
       <c r="B194" s="3"/>
       <c r="C194" s="2"/>
@@ -7501,7 +7514,7 @@
       <c r="M194" s="2"/>
       <c r="N194" s="2"/>
     </row>
-    <row r="195" spans="1:14">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A195" s="2"/>
       <c r="B195" s="3"/>
       <c r="C195" s="2"/>
@@ -7517,7 +7530,7 @@
       <c r="M195" s="2"/>
       <c r="N195" s="2"/>
     </row>
-    <row r="196" spans="1:14">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A196" s="2"/>
       <c r="B196" s="3"/>
       <c r="C196" s="2"/>
@@ -7533,7 +7546,7 @@
       <c r="M196" s="2"/>
       <c r="N196" s="2"/>
     </row>
-    <row r="197" spans="1:14">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A197" s="2"/>
       <c r="B197" s="3"/>
       <c r="C197" s="2"/>
@@ -7549,7 +7562,7 @@
       <c r="M197" s="2"/>
       <c r="N197" s="2"/>
     </row>
-    <row r="198" spans="1:14">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A198" s="2"/>
       <c r="B198" s="3"/>
       <c r="C198" s="2"/>
@@ -7565,7 +7578,7 @@
       <c r="M198" s="2"/>
       <c r="N198" s="2"/>
     </row>
-    <row r="199" spans="1:14">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A199" s="2"/>
       <c r="B199" s="3"/>
       <c r="C199" s="2"/>
@@ -7581,7 +7594,7 @@
       <c r="M199" s="2"/>
       <c r="N199" s="2"/>
     </row>
-    <row r="200" spans="1:14">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A200" s="2"/>
       <c r="B200" s="3"/>
       <c r="C200" s="2"/>
@@ -7597,7 +7610,7 @@
       <c r="M200" s="2"/>
       <c r="N200" s="2"/>
     </row>
-    <row r="201" spans="1:14">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A201" s="2"/>
       <c r="B201" s="3"/>
       <c r="C201" s="2"/>
@@ -7613,7 +7626,7 @@
       <c r="M201" s="2"/>
       <c r="N201" s="2"/>
     </row>
-    <row r="202" spans="1:14">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A202" s="2"/>
       <c r="B202" s="3"/>
       <c r="C202" s="2"/>
@@ -7629,7 +7642,7 @@
       <c r="M202" s="2"/>
       <c r="N202" s="2"/>
     </row>
-    <row r="203" spans="1:14">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A203" s="2"/>
       <c r="B203" s="3"/>
       <c r="C203" s="2"/>
@@ -7645,7 +7658,7 @@
       <c r="M203" s="2"/>
       <c r="N203" s="2"/>
     </row>
-    <row r="204" spans="1:14">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A204" s="2"/>
       <c r="B204" s="3"/>
       <c r="C204" s="2"/>
@@ -7661,7 +7674,7 @@
       <c r="M204" s="2"/>
       <c r="N204" s="2"/>
     </row>
-    <row r="205" spans="1:14">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A205" s="2"/>
       <c r="B205" s="3"/>
       <c r="C205" s="2"/>
@@ -7677,7 +7690,7 @@
       <c r="M205" s="2"/>
       <c r="N205" s="2"/>
     </row>
-    <row r="206" spans="1:14">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A206" s="2"/>
       <c r="B206" s="3"/>
       <c r="C206" s="2"/>
@@ -7693,7 +7706,7 @@
       <c r="M206" s="2"/>
       <c r="N206" s="2"/>
     </row>
-    <row r="207" spans="1:14">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A207" s="2"/>
       <c r="B207" s="3"/>
       <c r="C207" s="2"/>
@@ -7709,7 +7722,7 @@
       <c r="M207" s="2"/>
       <c r="N207" s="2"/>
     </row>
-    <row r="208" spans="1:14">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A208" s="2"/>
       <c r="B208" s="3"/>
       <c r="C208" s="2"/>
@@ -7725,7 +7738,7 @@
       <c r="M208" s="2"/>
       <c r="N208" s="2"/>
     </row>
-    <row r="209" spans="1:14">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A209" s="2"/>
       <c r="B209" s="3"/>
       <c r="C209" s="2"/>
@@ -7741,7 +7754,7 @@
       <c r="M209" s="2"/>
       <c r="N209" s="2"/>
     </row>
-    <row r="210" spans="1:14">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210" s="2"/>
       <c r="B210" s="3"/>
       <c r="C210" s="2"/>
@@ -7757,7 +7770,7 @@
       <c r="M210" s="2"/>
       <c r="N210" s="2"/>
     </row>
-    <row r="211" spans="1:14">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211" s="2"/>
       <c r="B211" s="3"/>
       <c r="C211" s="2"/>
@@ -7773,7 +7786,7 @@
       <c r="M211" s="2"/>
       <c r="N211" s="2"/>
     </row>
-    <row r="212" spans="1:14">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A212" s="2"/>
       <c r="B212" s="3"/>
       <c r="C212" s="2"/>
@@ -7789,7 +7802,7 @@
       <c r="M212" s="2"/>
       <c r="N212" s="2"/>
     </row>
-    <row r="213" spans="1:14">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213" s="2"/>
       <c r="B213" s="3"/>
       <c r="C213" s="2"/>
@@ -7805,7 +7818,7 @@
       <c r="M213" s="2"/>
       <c r="N213" s="2"/>
     </row>
-    <row r="214" spans="1:14">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A214" s="2"/>
       <c r="B214" s="3"/>
       <c r="C214" s="2"/>
@@ -7821,7 +7834,7 @@
       <c r="M214" s="2"/>
       <c r="N214" s="2"/>
     </row>
-    <row r="215" spans="1:14">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A215" s="2"/>
       <c r="B215" s="3"/>
       <c r="C215" s="2"/>
@@ -7837,7 +7850,7 @@
       <c r="M215" s="2"/>
       <c r="N215" s="2"/>
     </row>
-    <row r="216" spans="1:14">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A216" s="2"/>
       <c r="B216" s="3"/>
       <c r="C216" s="2"/>
@@ -7853,7 +7866,7 @@
       <c r="M216" s="2"/>
       <c r="N216" s="2"/>
     </row>
-    <row r="217" spans="1:14">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A217" s="2"/>
       <c r="B217" s="3"/>
       <c r="C217" s="2"/>
@@ -7869,7 +7882,7 @@
       <c r="M217" s="2"/>
       <c r="N217" s="2"/>
     </row>
-    <row r="218" spans="1:14">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A218" s="2"/>
       <c r="B218" s="3"/>
       <c r="C218" s="2"/>
@@ -7885,7 +7898,7 @@
       <c r="M218" s="2"/>
       <c r="N218" s="2"/>
     </row>
-    <row r="219" spans="1:14">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A219" s="2"/>
       <c r="B219" s="3"/>
       <c r="C219" s="2"/>
@@ -7901,7 +7914,7 @@
       <c r="M219" s="2"/>
       <c r="N219" s="2"/>
     </row>
-    <row r="220" spans="1:14">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A220" s="2"/>
       <c r="B220" s="3"/>
       <c r="C220" s="2"/>
@@ -7917,7 +7930,7 @@
       <c r="M220" s="2"/>
       <c r="N220" s="2"/>
     </row>
-    <row r="221" spans="1:14">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A221" s="2"/>
       <c r="B221" s="3"/>
       <c r="C221" s="2"/>
@@ -7933,7 +7946,7 @@
       <c r="M221" s="2"/>
       <c r="N221" s="2"/>
     </row>
-    <row r="222" spans="1:14">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A222" s="2"/>
       <c r="B222" s="3"/>
       <c r="C222" s="2"/>
@@ -7949,7 +7962,7 @@
       <c r="M222" s="2"/>
       <c r="N222" s="2"/>
     </row>
-    <row r="223" spans="1:14">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A223" s="2"/>
       <c r="B223" s="3"/>
       <c r="C223" s="2"/>
@@ -7965,7 +7978,7 @@
       <c r="M223" s="2"/>
       <c r="N223" s="2"/>
     </row>
-    <row r="224" spans="1:14">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A224" s="2"/>
       <c r="B224" s="3"/>
       <c r="C224" s="2"/>
@@ -7981,7 +7994,7 @@
       <c r="M224" s="2"/>
       <c r="N224" s="2"/>
     </row>
-    <row r="225" spans="1:14">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A225" s="2"/>
       <c r="B225" s="3"/>
       <c r="C225" s="2"/>
@@ -7997,7 +8010,7 @@
       <c r="M225" s="2"/>
       <c r="N225" s="2"/>
     </row>
-    <row r="226" spans="1:14">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A226" s="2"/>
       <c r="B226" s="3"/>
       <c r="C226" s="2"/>
@@ -8013,7 +8026,7 @@
       <c r="M226" s="2"/>
       <c r="N226" s="2"/>
     </row>
-    <row r="227" spans="1:14">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A227" s="2"/>
       <c r="B227" s="3"/>
       <c r="C227" s="2"/>
@@ -8029,7 +8042,7 @@
       <c r="M227" s="2"/>
       <c r="N227" s="2"/>
     </row>
-    <row r="228" spans="1:14">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
       <c r="B228" s="3"/>
       <c r="C228" s="2"/>
@@ -8045,7 +8058,7 @@
       <c r="M228" s="2"/>
       <c r="N228" s="2"/>
     </row>
-    <row r="229" spans="1:14">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A229" s="2"/>
       <c r="B229" s="3"/>
       <c r="C229" s="2"/>
@@ -8061,7 +8074,7 @@
       <c r="M229" s="2"/>
       <c r="N229" s="2"/>
     </row>
-    <row r="230" spans="1:14">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A230" s="2"/>
       <c r="B230" s="3"/>
       <c r="C230" s="2"/>
@@ -8077,7 +8090,7 @@
       <c r="M230" s="2"/>
       <c r="N230" s="2"/>
     </row>
-    <row r="231" spans="1:14">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A231" s="2"/>
       <c r="B231" s="3"/>
       <c r="C231" s="2"/>
@@ -8093,7 +8106,7 @@
       <c r="M231" s="2"/>
       <c r="N231" s="2"/>
     </row>
-    <row r="232" spans="1:14">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A232" s="2"/>
       <c r="B232" s="3"/>
       <c r="C232" s="2"/>
@@ -8109,7 +8122,7 @@
       <c r="M232" s="2"/>
       <c r="N232" s="2"/>
     </row>
-    <row r="233" spans="1:14">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A233" s="2"/>
       <c r="B233" s="3"/>
       <c r="C233" s="2"/>
@@ -8125,7 +8138,7 @@
       <c r="M233" s="2"/>
       <c r="N233" s="2"/>
     </row>
-    <row r="234" spans="1:14">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A234" s="2"/>
       <c r="B234" s="3"/>
       <c r="C234" s="2"/>
@@ -8141,7 +8154,7 @@
       <c r="M234" s="2"/>
       <c r="N234" s="2"/>
     </row>
-    <row r="235" spans="1:14">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A235" s="2"/>
       <c r="B235" s="3"/>
       <c r="C235" s="2"/>
@@ -8157,7 +8170,7 @@
       <c r="M235" s="2"/>
       <c r="N235" s="2"/>
     </row>
-    <row r="236" spans="1:14">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A236" s="2"/>
       <c r="B236" s="3"/>
       <c r="C236" s="2"/>
@@ -8173,7 +8186,7 @@
       <c r="M236" s="2"/>
       <c r="N236" s="2"/>
     </row>
-    <row r="237" spans="1:14">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A237" s="2"/>
       <c r="B237" s="3"/>
       <c r="C237" s="2"/>
@@ -8189,7 +8202,7 @@
       <c r="M237" s="2"/>
       <c r="N237" s="2"/>
     </row>
-    <row r="238" spans="1:14">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A238" s="2"/>
       <c r="B238" s="3"/>
       <c r="C238" s="2"/>
@@ -8205,7 +8218,7 @@
       <c r="M238" s="2"/>
       <c r="N238" s="2"/>
     </row>
-    <row r="239" spans="1:14">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A239" s="2"/>
       <c r="B239" s="3"/>
       <c r="C239" s="2"/>
@@ -8221,7 +8234,7 @@
       <c r="M239" s="2"/>
       <c r="N239" s="2"/>
     </row>
-    <row r="240" spans="1:14">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A240" s="2"/>
       <c r="B240" s="3"/>
       <c r="C240" s="2"/>
@@ -8237,7 +8250,7 @@
       <c r="M240" s="2"/>
       <c r="N240" s="2"/>
     </row>
-    <row r="241" spans="1:14">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A241" s="2"/>
       <c r="B241" s="3"/>
       <c r="C241" s="2"/>
@@ -8253,7 +8266,7 @@
       <c r="M241" s="2"/>
       <c r="N241" s="2"/>
     </row>
-    <row r="242" spans="1:14">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A242" s="2"/>
       <c r="B242" s="3"/>
       <c r="C242" s="2"/>
@@ -8269,7 +8282,7 @@
       <c r="M242" s="2"/>
       <c r="N242" s="2"/>
     </row>
-    <row r="243" spans="1:14">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A243" s="2"/>
       <c r="B243" s="3"/>
       <c r="C243" s="2"/>
@@ -8285,7 +8298,7 @@
       <c r="M243" s="2"/>
       <c r="N243" s="2"/>
     </row>
-    <row r="244" spans="1:14">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A244" s="2"/>
       <c r="B244" s="3"/>
       <c r="C244" s="2"/>
@@ -8301,7 +8314,7 @@
       <c r="M244" s="2"/>
       <c r="N244" s="2"/>
     </row>
-    <row r="245" spans="1:14">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A245" s="2"/>
       <c r="B245" s="3"/>
       <c r="C245" s="2"/>
@@ -8317,7 +8330,7 @@
       <c r="M245" s="2"/>
       <c r="N245" s="2"/>
     </row>
-    <row r="246" spans="1:14">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A246" s="2"/>
       <c r="B246" s="3"/>
       <c r="C246" s="2"/>
@@ -8333,7 +8346,7 @@
       <c r="M246" s="2"/>
       <c r="N246" s="2"/>
     </row>
-    <row r="247" spans="1:14">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A247" s="2"/>
       <c r="B247" s="3"/>
       <c r="C247" s="2"/>
@@ -8349,7 +8362,7 @@
       <c r="M247" s="2"/>
       <c r="N247" s="2"/>
     </row>
-    <row r="248" spans="1:14">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A248" s="2"/>
       <c r="B248" s="3"/>
       <c r="C248" s="2"/>
@@ -8365,7 +8378,7 @@
       <c r="M248" s="2"/>
       <c r="N248" s="2"/>
     </row>
-    <row r="249" spans="1:14">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A249" s="2"/>
       <c r="B249" s="3"/>
       <c r="C249" s="2"/>
@@ -8381,7 +8394,7 @@
       <c r="M249" s="2"/>
       <c r="N249" s="2"/>
     </row>
-    <row r="250" spans="1:14">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A250" s="2"/>
       <c r="B250" s="3"/>
       <c r="C250" s="2"/>
@@ -8397,7 +8410,7 @@
       <c r="M250" s="2"/>
       <c r="N250" s="2"/>
     </row>
-    <row r="251" spans="1:14">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A251" s="2"/>
       <c r="B251" s="3"/>
       <c r="C251" s="2"/>
@@ -8413,7 +8426,7 @@
       <c r="M251" s="2"/>
       <c r="N251" s="2"/>
     </row>
-    <row r="252" spans="1:14">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A252" s="2"/>
       <c r="B252" s="3"/>
       <c r="C252" s="2"/>
@@ -8429,7 +8442,7 @@
       <c r="M252" s="2"/>
       <c r="N252" s="2"/>
     </row>
-    <row r="253" spans="1:14">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A253" s="2"/>
       <c r="B253" s="3"/>
       <c r="C253" s="2"/>
@@ -8445,7 +8458,7 @@
       <c r="M253" s="2"/>
       <c r="N253" s="2"/>
     </row>
-    <row r="254" spans="1:14">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A254" s="2"/>
       <c r="B254" s="3"/>
       <c r="C254" s="2"/>
@@ -8461,7 +8474,7 @@
       <c r="M254" s="2"/>
       <c r="N254" s="2"/>
     </row>
-    <row r="255" spans="1:14">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A255" s="2"/>
       <c r="B255" s="3"/>
       <c r="C255" s="2"/>
@@ -8477,7 +8490,7 @@
       <c r="M255" s="2"/>
       <c r="N255" s="2"/>
     </row>
-    <row r="256" spans="1:14">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A256" s="2"/>
       <c r="B256" s="3"/>
       <c r="C256" s="2"/>
@@ -8493,7 +8506,7 @@
       <c r="M256" s="2"/>
       <c r="N256" s="2"/>
     </row>
-    <row r="257" spans="1:14">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A257" s="2"/>
       <c r="B257" s="3"/>
       <c r="C257" s="2"/>

</xml_diff>